<commit_message>
refactor: editado valores da tabela
</commit_message>
<xml_diff>
--- a/Catalogo-Tabela-Bitolas-Editado-2.xlsx
+++ b/Catalogo-Tabela-Bitolas-Editado-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26f55fd51023be96/Documentos/Faculdade Mauá/3. Iniciação/Scripts/confiabilidade-viga-mista/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzo/Documents/Development/confiabilidade-viga-mista/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="14_{9E26C696-11D6-4980-A2F5-6FDDEBF68C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E61BB7D6-0A27-48CF-B716-236758E5230A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7298C1-65E9-644B-A560-8427DD1245B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DE063C6D-B184-4314-87E3-CEB7A007B528}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{DE063C6D-B184-4314-87E3-CEB7A007B528}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFIS_ESTRUTURAIS_W_E_HP" sheetId="3" r:id="rId1"/>
@@ -63,18 +63,6 @@
     <t>d</t>
   </si>
   <si>
-    <t xml:space="preserve">h </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa </t>
-  </si>
-  <si>
     <t>Alma</t>
   </si>
   <si>
@@ -92,38 +80,6 @@
   </si>
   <si>
     <t>massa_linear</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>tf</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="4.5"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>mm</t>
-    </r>
   </si>
   <si>
     <t>Ix</t>
@@ -155,15 +111,30 @@
   <si>
     <t>Cw</t>
   </si>
+  <si>
+    <t>tf</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>d'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,20 +156,6 @@
     <font>
       <sz val="7"/>
       <color rgb="FF003E74"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="subscript"/>
-      <sz val="4.5"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -291,10 +248,10 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,7 +260,7 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,7 +269,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -321,7 +278,7 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -330,7 +287,7 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -357,14 +314,14 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,10 +338,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,81 +639,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86DAE0C-D401-4FE2-A997-BAF16F0E390B}">
   <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="N1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="U1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>13</v>
       </c>
@@ -828,7 +781,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>18</v>
       </c>
@@ -896,7 +849,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>22.5</v>
       </c>
@@ -964,7 +917,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>24</v>
       </c>
@@ -1032,7 +985,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>29.8</v>
       </c>
@@ -1100,7 +1053,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>37.1</v>
       </c>
@@ -1168,7 +1121,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>15</v>
       </c>
@@ -1236,7 +1189,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>19.3</v>
       </c>
@@ -1304,7 +1257,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>22.5</v>
       </c>
@@ -1372,7 +1325,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>26.6</v>
       </c>
@@ -1440,7 +1393,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>31.3</v>
       </c>
@@ -1508,7 +1461,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>35.9</v>
       </c>
@@ -1576,7 +1529,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>41.7</v>
       </c>
@@ -1644,7 +1597,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>46.1</v>
       </c>
@@ -1712,7 +1665,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>52</v>
       </c>
@@ -1780,7 +1733,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>53</v>
       </c>
@@ -1848,7 +1801,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>59</v>
       </c>
@@ -1916,7 +1869,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>71</v>
       </c>
@@ -1984,7 +1937,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>86</v>
       </c>
@@ -2052,7 +2005,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>100</v>
       </c>
@@ -2120,7 +2073,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>17.899999999999999</v>
       </c>
@@ -2188,7 +2141,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22.3</v>
       </c>
@@ -2256,7 +2209,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>25.3</v>
       </c>
@@ -2324,7 +2277,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>28.4</v>
       </c>
@@ -2392,7 +2345,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>32.700000000000003</v>
       </c>
@@ -2460,7 +2413,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>38.5</v>
       </c>
@@ -2528,7 +2481,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>44.8</v>
       </c>
@@ -2596,7 +2549,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>62</v>
       </c>
@@ -2664,7 +2617,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>73</v>
       </c>
@@ -2732,7 +2685,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>80</v>
       </c>
@@ -2800,7 +2753,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>85</v>
       </c>
@@ -2868,7 +2821,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>89</v>
       </c>
@@ -2936,7 +2889,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>101</v>
       </c>
@@ -3004,7 +2957,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>115</v>
       </c>
@@ -3072,7 +3025,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>131</v>
       </c>
@@ -3140,7 +3093,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>149</v>
       </c>
@@ -3208,7 +3161,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <v>167</v>
       </c>
@@ -3276,7 +3229,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="16">
         <v>21</v>
       </c>
@@ -3344,7 +3297,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>23.8</v>
       </c>
@@ -3412,7 +3365,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>28.3</v>
       </c>
@@ -3480,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>32.700000000000003</v>
       </c>
@@ -3548,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>38.700000000000003</v>
       </c>
@@ -3616,7 +3569,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>44.5</v>
       </c>
@@ -3684,7 +3637,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>52</v>
       </c>
@@ -3752,7 +3705,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>60</v>
       </c>
@@ -3820,7 +3773,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>67</v>
       </c>
@@ -3888,7 +3841,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>74</v>
       </c>
@@ -3956,7 +3909,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>79</v>
       </c>
@@ -4024,7 +3977,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>93</v>
       </c>
@@ -4092,7 +4045,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>97</v>
       </c>
@@ -4160,7 +4113,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>107</v>
       </c>
@@ -4228,7 +4181,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>110</v>
       </c>
@@ -4296,7 +4249,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>117</v>
       </c>
@@ -4364,7 +4317,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>125</v>
       </c>
@@ -4432,7 +4385,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>129</v>
       </c>
@@ -4500,7 +4453,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>132</v>
       </c>
@@ -4568,7 +4521,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>143</v>
       </c>
@@ -4636,7 +4589,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>158</v>
       </c>
@@ -4704,7 +4657,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>179</v>
       </c>
@@ -4772,7 +4725,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>202</v>
       </c>
@@ -4840,7 +4793,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>32.9</v>
       </c>
@@ -4908,7 +4861,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>39</v>
       </c>
@@ -4976,7 +4929,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>44.6</v>
       </c>
@@ -5044,7 +4997,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>51</v>
       </c>
@@ -5112,7 +5065,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>58</v>
       </c>
@@ -5180,7 +5133,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -5248,7 +5201,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>72</v>
       </c>
@@ -5316,7 +5269,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>79</v>
       </c>
@@ -5384,7 +5337,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>91</v>
       </c>
@@ -5452,7 +5405,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>101</v>
       </c>
@@ -5520,7 +5473,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>110</v>
       </c>
@@ -5588,7 +5541,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>122</v>
       </c>
@@ -5656,7 +5609,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>38.799999999999997</v>
       </c>
@@ -5724,7 +5677,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>46.1</v>
       </c>
@@ -5792,7 +5745,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>53</v>
       </c>
@@ -5860,7 +5813,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>60</v>
       </c>
@@ -5928,7 +5881,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>67</v>
       </c>
@@ -5996,7 +5949,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -6064,7 +6017,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" s="13">
         <v>85</v>
       </c>
@@ -6132,7 +6085,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <v>52</v>
       </c>
@@ -6200,7 +6153,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>60</v>
       </c>
@@ -6268,7 +6221,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>68</v>
       </c>
@@ -6336,7 +6289,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>74</v>
       </c>
@@ -6397,14 +6350,14 @@
       <c r="T84" s="1">
         <v>44.89</v>
       </c>
-      <c r="U84" s="27" t="s">
+      <c r="U84" s="26" t="s">
         <v>0</v>
       </c>
       <c r="V84" s="1">
         <v>1.64</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>82</v>
       </c>
@@ -6472,7 +6425,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>89</v>
       </c>
@@ -6540,7 +6493,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>97</v>
       </c>
@@ -6608,7 +6561,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" s="13">
         <v>106</v>
       </c>
@@ -6676,7 +6629,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>66</v>
       </c>
@@ -6744,7 +6697,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>72</v>
       </c>
@@ -6812,7 +6765,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>74</v>
       </c>
@@ -6880,7 +6833,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>82</v>
       </c>
@@ -6948,7 +6901,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>85</v>
       </c>
@@ -7016,7 +6969,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>92</v>
       </c>
@@ -7084,7 +7037,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>101</v>
       </c>
@@ -7152,7 +7105,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>109</v>
       </c>
@@ -7220,7 +7173,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>123</v>
       </c>
@@ -7288,7 +7241,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98" s="13">
         <v>138</v>
       </c>
@@ -7356,7 +7309,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99" s="16">
         <v>82</v>
       </c>
@@ -7424,7 +7377,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>92</v>
       </c>
@@ -7492,7 +7445,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>101</v>
       </c>
@@ -7560,7 +7513,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>113</v>
       </c>
@@ -7628,7 +7581,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>125</v>
       </c>
@@ -7696,7 +7649,7 @@
         <v>2.09</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>140</v>
       </c>
@@ -7764,7 +7717,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>154.19999999999999</v>
       </c>
@@ -7832,7 +7785,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>155</v>
       </c>
@@ -7900,7 +7853,7 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>174</v>
       </c>
@@ -7968,7 +7921,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>195</v>
       </c>
@@ -8014,7 +7967,7 @@
       <c r="O108" s="1">
         <v>7.55</v>
       </c>
-      <c r="P108" s="27" t="s">
+      <c r="P108" s="26" t="s">
         <v>1</v>
       </c>
       <c r="Q108" s="1">
@@ -8036,7 +7989,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>217</v>
       </c>

</xml_diff>